<commit_message>
added totalAmount of generated reports
</commit_message>
<xml_diff>
--- a/server/public/templates/reports_2023-10-10.xlsx
+++ b/server/public/templates/reports_2023-10-10.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Kryzz Andig</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
@@ -547,6 +550,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>70000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>